<commit_message>
completed delivery idea 1 and progress on circuit
*finished first draft of delivery idea 1
*started delivery idea 2
*made progress on circuit
*finished schematic
*half way through layout
</commit_message>
<xml_diff>
--- a/Circuit/Part List.xlsx
+++ b/Circuit/Part List.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="137">
   <si>
     <t>component</t>
   </si>
@@ -377,6 +377,66 @@
   </si>
   <si>
     <t>per metre</t>
+  </si>
+  <si>
+    <t>A4988 Braekout board</t>
+  </si>
+  <si>
+    <t>2A stepper motor driver</t>
+  </si>
+  <si>
+    <t>communica</t>
+  </si>
+  <si>
+    <t>Quantity</t>
+  </si>
+  <si>
+    <t>1k ohm res</t>
+  </si>
+  <si>
+    <t>10k ohm res</t>
+  </si>
+  <si>
+    <t>4 way one way header</t>
+  </si>
+  <si>
+    <t>3 way header</t>
+  </si>
+  <si>
+    <t>6 way one way header</t>
+  </si>
+  <si>
+    <t>friction lock one way header</t>
+  </si>
+  <si>
+    <t>standard header pins</t>
+  </si>
+  <si>
+    <t>8 way socket</t>
+  </si>
+  <si>
+    <t>2.54 pitch</t>
+  </si>
+  <si>
+    <t>DIP</t>
+  </si>
+  <si>
+    <t>Cable</t>
+  </si>
+  <si>
+    <t>Breakout</t>
+  </si>
+  <si>
+    <t>10pF cap</t>
+  </si>
+  <si>
+    <t>chip capacitor</t>
+  </si>
+  <si>
+    <t>Other</t>
+  </si>
+  <si>
+    <t>total</t>
   </si>
 </sst>
 </file>
@@ -485,7 +545,7 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="3" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="3" applyFill="1" applyAlignment="1">
@@ -497,6 +557,9 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="4" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -1152,535 +1215,805 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:M20"/>
+  <dimension ref="B2:V29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" thickTop="1" thickBottom="1" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="16.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="31.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.85546875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="8" width="12.7109375" style="1" customWidth="1"/>
-    <col min="9" max="9" width="11.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.140625" style="1" customWidth="1"/>
-    <col min="11" max="11" width="12.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="16384" width="9.140625" style="1"/>
+    <col min="3" max="3" width="25" style="1" customWidth="1"/>
+    <col min="4" max="4" width="31.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.85546875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="10" width="12.7109375" style="1" customWidth="1"/>
+    <col min="11" max="11" width="11.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.140625" style="1" customWidth="1"/>
+    <col min="13" max="13" width="12.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="16" width="9.140625" style="1"/>
+    <col min="17" max="17" width="11.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:13" ht="24.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="2:22" ht="24.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B2" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="C2" s="3"/>
+      <c r="G2" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="M2" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="L2" s="1">
+      <c r="N2" s="1">
         <v>14.18</v>
       </c>
-      <c r="M2" s="1" t="s">
+      <c r="O2" s="1" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="4" spans="2:13" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:22" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="1" t="s">
         <v>60</v>
       </c>
       <c r="C4" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="E4" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="F4" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="G4" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="H4" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="H4" s="1" t="s">
+      <c r="I4" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="I4" s="1" t="s">
+      <c r="J4" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="K4" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="J4" s="1" t="s">
+      <c r="L4" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="K4" s="1" t="s">
+      <c r="M4" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="L4" s="1" t="s">
+      <c r="N4" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="M4" s="1" t="s">
+      <c r="O4" s="1" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="5" spans="2:13" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="P4" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="Q4" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="R4" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="S4" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="T4" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="U4" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="V4" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="5" spans="2:22" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" s="1">
+        <v>1</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="E5" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="F5" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="F5" s="4">
+      <c r="G5" s="4">
         <v>0</v>
       </c>
-      <c r="G5" s="4" t="s">
+      <c r="H5" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="H5" s="4"/>
-      <c r="I5" s="5" t="s">
+      <c r="I5" s="4"/>
+      <c r="J5" s="4"/>
+      <c r="K5" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="J5" s="1">
+      <c r="L5" s="1">
         <v>1</v>
       </c>
-      <c r="K5" s="1">
+      <c r="M5" s="1">
         <v>2.71</v>
       </c>
-      <c r="L5" s="1">
-        <f>K5*$L$2</f>
+      <c r="N5" s="1">
+        <f>M5*$N$2</f>
         <v>38.427799999999998</v>
       </c>
-      <c r="M5" s="1">
-        <f>L5/J5</f>
+      <c r="O5" s="1">
+        <f>N5/L5</f>
         <v>38.427799999999998</v>
       </c>
     </row>
-    <row r="6" spans="2:13" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:22" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" s="1">
+        <v>1</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="D6" s="7" t="s">
+      <c r="E6" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="E6" s="5" t="s">
+      <c r="F6" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="F6" s="1">
+      <c r="G6" s="1">
         <v>10</v>
       </c>
-      <c r="G6" s="1">
+      <c r="H6" s="1">
         <v>89.66</v>
       </c>
-      <c r="H6" s="1">
-        <f>G6/F6</f>
+      <c r="I6" s="1">
+        <f>H6/G6</f>
         <v>8.9659999999999993</v>
       </c>
-      <c r="I6" s="5" t="s">
+      <c r="K6" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="J6" s="1">
+      <c r="L6" s="1">
         <v>1</v>
       </c>
-      <c r="K6" s="1">
+      <c r="M6" s="1">
         <v>0.77</v>
       </c>
-      <c r="L6" s="1">
-        <f t="shared" ref="L6:L19" si="0">K6*$L$2</f>
+      <c r="N6" s="1">
+        <f t="shared" ref="N6:N20" si="0">M6*$N$2</f>
         <v>10.9186</v>
       </c>
-      <c r="M6" s="1">
-        <f t="shared" ref="M6:M19" si="1">L6/J6</f>
+      <c r="O6" s="1">
+        <f t="shared" ref="O6:O26" si="1">N6/L6</f>
         <v>10.9186</v>
       </c>
     </row>
-    <row r="7" spans="2:13" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:22" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="D7" s="7" t="s">
+      <c r="C7" s="1">
+        <v>1</v>
+      </c>
+      <c r="E7" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="E7" s="5" t="s">
+      <c r="F7" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="F7" s="1">
+      <c r="G7" s="1">
         <v>10</v>
       </c>
-      <c r="G7" s="1">
+      <c r="H7" s="1">
         <v>29.82</v>
       </c>
-      <c r="H7" s="1">
-        <f t="shared" ref="H7:H16" si="2">G7/F7</f>
+      <c r="I7" s="1">
+        <f t="shared" ref="I7:I26" si="2">H7/G7</f>
         <v>2.9820000000000002</v>
       </c>
-      <c r="I7" s="5" t="s">
+      <c r="K7" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="J7" s="1">
+      <c r="L7" s="1">
         <v>1</v>
       </c>
-      <c r="K7" s="1">
+      <c r="M7" s="1">
         <v>0.27</v>
       </c>
-      <c r="L7" s="1">
+      <c r="N7" s="1">
         <f t="shared" si="0"/>
         <v>3.8286000000000002</v>
       </c>
-      <c r="M7" s="1">
+      <c r="O7" s="1">
         <f t="shared" si="1"/>
         <v>3.8286000000000002</v>
       </c>
     </row>
-    <row r="8" spans="2:13" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:22" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="C8" s="1">
+        <v>2</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="E8" s="7">
+        <v>805</v>
+      </c>
+      <c r="F8" s="5"/>
+      <c r="K8" s="5"/>
+    </row>
+    <row r="9" spans="2:22" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C9" s="1">
+        <v>1</v>
+      </c>
+      <c r="D9" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="D8" s="7">
+      <c r="E9" s="7">
         <v>805</v>
       </c>
-      <c r="E8" s="5" t="s">
+      <c r="F9" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="F8" s="1">
+      <c r="G9" s="1">
         <v>50</v>
       </c>
-      <c r="G8" s="1">
+      <c r="H9" s="1">
         <v>6.55</v>
       </c>
-      <c r="H8" s="1">
+      <c r="I9" s="1">
         <f t="shared" si="2"/>
         <v>0.13100000000000001</v>
       </c>
-      <c r="I8" s="5" t="s">
+      <c r="K9" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="J8" s="1">
+      <c r="L9" s="1">
         <v>1</v>
       </c>
-      <c r="K8" s="1">
+      <c r="M9" s="1">
         <v>0.1</v>
       </c>
-      <c r="L8" s="1">
+      <c r="N9" s="1">
         <f t="shared" si="0"/>
         <v>1.4180000000000001</v>
       </c>
-      <c r="M8" s="1">
+      <c r="O9" s="1">
         <f t="shared" si="1"/>
         <v>1.4180000000000001</v>
       </c>
     </row>
-    <row r="9" spans="2:13" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="1" t="s">
+    <row r="10" spans="2:22" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C10" s="1">
+        <v>2</v>
+      </c>
+      <c r="D10" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="D9" s="7" t="s">
+      <c r="E10" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="F10" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="F9" s="1">
+      <c r="G10" s="1">
         <v>25</v>
       </c>
-      <c r="G9" s="1">
+      <c r="H10" s="1">
         <v>10.475</v>
       </c>
-      <c r="H9" s="1">
+      <c r="I10" s="1">
         <f t="shared" si="2"/>
         <v>0.41899999999999998</v>
       </c>
-      <c r="I9" s="1" t="s">
+      <c r="K10" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="J9" s="1">
+      <c r="L10" s="1">
         <v>1</v>
       </c>
-      <c r="K9" s="1">
+      <c r="M10" s="1">
         <v>0.1</v>
       </c>
-      <c r="L9" s="1">
+      <c r="N10" s="1">
         <f t="shared" si="0"/>
         <v>1.4180000000000001</v>
       </c>
-      <c r="M9" s="1">
-        <f t="shared" si="1"/>
+      <c r="O10" s="1">
+        <f>N10*L10</f>
         <v>1.4180000000000001</v>
       </c>
     </row>
-    <row r="10" spans="2:13" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="1" t="s">
+    <row r="11" spans="2:22" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C11" s="1">
+        <v>2</v>
+      </c>
+      <c r="D11" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="D10" s="7" t="s">
+      <c r="E11" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="H10" s="1" t="e">
+      <c r="I11" s="1" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="I10" s="1" t="s">
+      <c r="K11" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="J10" s="1">
+      <c r="L11" s="1">
         <v>1</v>
       </c>
-      <c r="K10" s="1">
+      <c r="M11" s="1">
         <v>0.14000000000000001</v>
       </c>
-      <c r="L10" s="1">
+      <c r="N11" s="1">
         <f t="shared" si="0"/>
         <v>1.9852000000000001</v>
       </c>
-      <c r="M10" s="1">
+      <c r="O11" s="1">
         <f t="shared" si="1"/>
         <v>1.9852000000000001</v>
       </c>
     </row>
-    <row r="11" spans="2:13" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="1" t="s">
+    <row r="12" spans="2:22" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C12" s="1">
+        <v>1</v>
+      </c>
+      <c r="D12" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="D11" s="7"/>
-      <c r="H11" s="1" t="e">
+      <c r="E12" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="I12" s="1" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="I11" s="1" t="s">
+      <c r="K12" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="J11" s="1">
+      <c r="L12" s="1">
         <v>1</v>
       </c>
-      <c r="K11" s="1">
+      <c r="M12" s="1">
         <v>0.91</v>
       </c>
-      <c r="L11" s="1">
+      <c r="N12" s="1">
         <f t="shared" si="0"/>
         <v>12.9038</v>
       </c>
-      <c r="M11" s="1">
+      <c r="O12" s="1">
         <f t="shared" si="1"/>
         <v>12.9038</v>
       </c>
     </row>
-    <row r="12" spans="2:13" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="1" t="s">
+    <row r="13" spans="2:22" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="C13" s="1">
+        <v>5</v>
+      </c>
+      <c r="D13" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="D12" s="7">
+      <c r="E13" s="7">
         <v>805</v>
       </c>
-      <c r="H12" s="1" t="e">
+      <c r="I13" s="1" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="L12" s="1">
+      <c r="N13" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="M12" s="1" t="e">
+      <c r="O13" s="1" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="13" spans="2:13" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="1" t="s">
+    <row r="14" spans="2:22" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="C14" s="1">
+        <v>3</v>
+      </c>
+      <c r="D14" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="D13" s="7">
+      <c r="E14" s="7">
         <v>805</v>
       </c>
-      <c r="H13" s="1" t="e">
+      <c r="I14" s="1" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="L13" s="1">
+      <c r="N14" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="M13" s="1" t="e">
+      <c r="O14" s="1" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="14" spans="2:13" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="1" t="s">
+    <row r="15" spans="2:22" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="D14" s="7">
+      <c r="C15" s="1">
+        <v>1</v>
+      </c>
+      <c r="E15" s="7">
         <v>1206</v>
       </c>
-      <c r="H14" s="1" t="e">
+      <c r="I15" s="1" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="L14" s="1">
+      <c r="N15" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="M14" s="1" t="e">
+      <c r="O15" s="1" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="15" spans="2:13" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="1" t="s">
+    <row r="16" spans="2:22" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="D15" s="7">
+      <c r="C16" s="1">
+        <v>1</v>
+      </c>
+      <c r="E16" s="7">
         <v>1206</v>
       </c>
-      <c r="H15" s="1" t="e">
+      <c r="I16" s="1" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="L15" s="1">
+      <c r="N16" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="M15" s="1" t="e">
+      <c r="O16" s="1" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="16" spans="2:13" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="1" t="s">
+    <row r="17" spans="2:21" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="D16" s="7">
+      <c r="C17" s="1">
+        <v>1</v>
+      </c>
+      <c r="E17" s="7">
         <v>1206</v>
       </c>
-      <c r="H16" s="1" t="e">
+      <c r="I17" s="1" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="L16" s="1">
+      <c r="N17" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="M16" s="1" t="e">
+      <c r="O17" s="1" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="17" spans="2:13" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="1" t="s">
+    <row r="18" spans="2:21" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="C18" s="1">
+        <v>1</v>
+      </c>
+      <c r="D18" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="D17" s="7">
+      <c r="E18" s="7">
         <v>805</v>
       </c>
-      <c r="L17" s="1">
+      <c r="I18" s="1" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N18" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="M17" s="1" t="e">
+      <c r="O18" s="1" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="18" spans="2:13" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="1" t="s">
+    <row r="19" spans="2:21" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="C18" s="1" t="s">
+      <c r="C19" s="1">
+        <v>3</v>
+      </c>
+      <c r="D19" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="D18" s="7">
+      <c r="E19" s="7">
         <v>805</v>
       </c>
-      <c r="L18" s="1">
+      <c r="I19" s="1" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N19" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="M18" s="1" t="e">
+      <c r="O19" s="1" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="19" spans="2:13" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="1" t="s">
+    <row r="20" spans="2:21" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="C20" s="1">
+        <v>2</v>
+      </c>
+      <c r="D20" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="D19" s="7">
+      <c r="E20" s="7">
         <v>805</v>
       </c>
-      <c r="L19" s="1">
+      <c r="I20" s="1" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N20" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="M19" s="1" t="e">
+      <c r="O20" s="1" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="20" spans="2:13" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="1" t="s">
+    <row r="21" spans="2:21" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B21" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="C21" s="1">
+        <v>3</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="E21" s="7">
+        <v>805</v>
+      </c>
+      <c r="I21" s="1" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O21" s="1" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="22" spans="2:21" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B22" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C22" s="1">
+        <v>2</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="E22" s="7">
+        <v>805</v>
+      </c>
+      <c r="I22" s="1" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O22" s="1" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="23" spans="2:21" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B23" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="C23" s="1">
+        <v>1</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="E23" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="I23" s="1" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O23" s="1" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="24" spans="2:21" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B24" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="C24" s="1">
+        <v>2</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="E24" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="I24" s="1" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O24" s="1" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="25" spans="2:21" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B25" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="C25" s="1">
+        <v>3</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="E25" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="I25" s="1" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O25" s="1" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="26" spans="2:21" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B26" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="C26" s="1">
+        <v>2</v>
+      </c>
+      <c r="E26" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="I26" s="1" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O26" s="1" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="27" spans="2:21" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B27" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="C20" s="1" t="s">
+      <c r="C27" s="1">
+        <v>1</v>
+      </c>
+      <c r="D27" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="D20" s="7"/>
-      <c r="E20" s="1" t="s">
+      <c r="E27" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="Q27" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="F20" s="1" t="s">
+      <c r="R27" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="G20" s="1">
+      <c r="T27" s="1">
         <v>8.64</v>
       </c>
-      <c r="M20" s="1">
+      <c r="U27" s="1">
         <v>8.64</v>
       </c>
+    </row>
+    <row r="28" spans="2:21" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B28" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="C28" s="1">
+        <v>1</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="E28" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="Q28" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="R28" s="1">
+        <v>1</v>
+      </c>
+      <c r="T28" s="1">
+        <v>59</v>
+      </c>
+      <c r="U28" s="1">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="29" spans="2:21" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E29" s="8"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E6" r:id="rId1"/>
-    <hyperlink ref="I8" r:id="rId2"/>
-    <hyperlink ref="I6" r:id="rId3"/>
-    <hyperlink ref="I5" r:id="rId4"/>
-    <hyperlink ref="E5"/>
-    <hyperlink ref="E7" r:id="rId5"/>
-    <hyperlink ref="E8" r:id="rId6"/>
+    <hyperlink ref="F6" r:id="rId1"/>
+    <hyperlink ref="K9" r:id="rId2"/>
+    <hyperlink ref="K6" r:id="rId3"/>
+    <hyperlink ref="K5" r:id="rId4"/>
+    <hyperlink ref="F5" display="http://za.rs-online.com/web/p/microcontrollers/7618633/?searchTerm=stm32f051c6t&amp;relevancy-data=636F3D3526696E3D4931384E4D616E506172744E756D626572266C753D656E266D6D3D6D61746368616C6C7061727469616C26706D3D5E5B5C707B4C7D5C707B4E647D2D2C2F255C2E5D2B2426706F3D"/>
+    <hyperlink ref="F7" r:id="rId5"/>
+    <hyperlink ref="F9" r:id="rId6"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
redid layout and updated document
updated the document and redid the layout to improve layout and added
more initilizaton to the document
</commit_message>
<xml_diff>
--- a/Circuit/Part List.xlsx
+++ b/Circuit/Part List.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="147">
   <si>
     <t>component</t>
   </si>
@@ -437,6 +437,36 @@
   </si>
   <si>
     <t>total</t>
+  </si>
+  <si>
+    <t>link</t>
+  </si>
+  <si>
+    <t>http://www.communica.co.za/Catalog/Details/P4013654006</t>
+  </si>
+  <si>
+    <t>for programming</t>
+  </si>
+  <si>
+    <t xml:space="preserve">red cable </t>
+  </si>
+  <si>
+    <t>high current cabling</t>
+  </si>
+  <si>
+    <t>csa=0.75</t>
+  </si>
+  <si>
+    <t>http://www.mantech.co.za/ProductInfo.aspx?Item=52M0039</t>
+  </si>
+  <si>
+    <t>grey cable</t>
+  </si>
+  <si>
+    <t>http://www.mantech.co.za/ProductInfo.aspx?Item=52M0036</t>
+  </si>
+  <si>
+    <t>permetre</t>
   </si>
 </sst>
 </file>
@@ -1215,10 +1245,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:V29"/>
+  <dimension ref="A2:W30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D37" sqref="D37"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="U31" sqref="U31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" thickTop="1" thickBottom="1" x14ac:dyDescent="0.3"/>
@@ -1235,10 +1265,11 @@
     <col min="13" max="13" width="12.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="14" max="16" width="9.140625" style="1"/>
     <col min="17" max="17" width="11.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="16384" width="9.140625" style="1"/>
+    <col min="18" max="18" width="11.140625" style="1" customWidth="1"/>
+    <col min="19" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:22" ht="24.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="2:23" ht="24.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B2" s="3" t="s">
         <v>59</v>
       </c>
@@ -1256,7 +1287,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="4" spans="2:22" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:23" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="1" t="s">
         <v>60</v>
       </c>
@@ -1306,22 +1337,25 @@
         <v>135</v>
       </c>
       <c r="R4" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="S4" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="S4" s="1" t="s">
+      <c r="T4" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="T4" s="1" t="s">
+      <c r="U4" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="U4" s="1" t="s">
+      <c r="V4" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="V4" s="1" t="s">
+      <c r="W4" s="1" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="5" spans="2:22" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:23" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="1" t="s">
         <v>64</v>
       </c>
@@ -1363,7 +1397,7 @@
         <v>38.427799999999998</v>
       </c>
     </row>
-    <row r="6" spans="2:22" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:23" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="1" t="s">
         <v>71</v>
       </c>
@@ -1407,7 +1441,7 @@
         <v>10.9186</v>
       </c>
     </row>
-    <row r="7" spans="2:22" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:23" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="1" t="s">
         <v>76</v>
       </c>
@@ -1448,7 +1482,7 @@
         <v>3.8286000000000002</v>
       </c>
     </row>
-    <row r="8" spans="2:22" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:23" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="1" t="s">
         <v>133</v>
       </c>
@@ -1464,7 +1498,7 @@
       <c r="F8" s="5"/>
       <c r="K8" s="5"/>
     </row>
-    <row r="9" spans="2:22" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:23" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B9" s="1" t="s">
         <v>85</v>
       </c>
@@ -1508,7 +1542,7 @@
         <v>1.4180000000000001</v>
       </c>
     </row>
-    <row r="10" spans="2:22" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:23" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B10" s="1" t="s">
         <v>92</v>
       </c>
@@ -1552,7 +1586,7 @@
         <v>1.4180000000000001</v>
       </c>
     </row>
-    <row r="11" spans="2:22" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:23" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B11" s="1" t="s">
         <v>95</v>
       </c>
@@ -1587,7 +1621,7 @@
         <v>1.9852000000000001</v>
       </c>
     </row>
-    <row r="12" spans="2:22" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:23" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B12" s="1" t="s">
         <v>99</v>
       </c>
@@ -1622,7 +1656,7 @@
         <v>12.9038</v>
       </c>
     </row>
-    <row r="13" spans="2:22" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:23" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B13" s="1" t="s">
         <v>104</v>
       </c>
@@ -1648,7 +1682,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="14" spans="2:22" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:23" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B14" s="1" t="s">
         <v>105</v>
       </c>
@@ -1674,7 +1708,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="15" spans="2:22" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:23" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B15" s="1" t="s">
         <v>106</v>
       </c>
@@ -1697,7 +1731,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="16" spans="2:22" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:23" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B16" s="1" t="s">
         <v>107</v>
       </c>
@@ -1720,7 +1754,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="17" spans="2:21" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:22" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B17" s="1" t="s">
         <v>108</v>
       </c>
@@ -1743,7 +1777,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="18" spans="2:21" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:22" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B18" s="1" t="s">
         <v>110</v>
       </c>
@@ -1769,7 +1803,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="19" spans="2:21" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:22" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B19" s="1" t="s">
         <v>111</v>
       </c>
@@ -1795,7 +1829,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="20" spans="2:21" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:22" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B20" s="1" t="s">
         <v>112</v>
       </c>
@@ -1821,7 +1855,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="21" spans="2:21" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:22" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B21" s="1" t="s">
         <v>121</v>
       </c>
@@ -1843,7 +1877,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="22" spans="2:21" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:22" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B22" s="1" t="s">
         <v>122</v>
       </c>
@@ -1865,7 +1899,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="23" spans="2:21" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:22" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B23" s="1" t="s">
         <v>124</v>
       </c>
@@ -1887,7 +1921,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="24" spans="2:21" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:22" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B24" s="1" t="s">
         <v>123</v>
       </c>
@@ -1909,7 +1943,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="25" spans="2:21" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:22" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B25" s="1" t="s">
         <v>125</v>
       </c>
@@ -1931,7 +1965,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="26" spans="2:21" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:22" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B26" s="1" t="s">
         <v>128</v>
       </c>
@@ -1950,7 +1984,10 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="27" spans="2:21" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:22" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="1" t="s">
+        <v>139</v>
+      </c>
       <c r="B27" s="1" t="s">
         <v>113</v>
       </c>
@@ -1966,17 +2003,17 @@
       <c r="Q27" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="R27" s="1" t="s">
+      <c r="S27" s="1" t="s">
         <v>116</v>
-      </c>
-      <c r="T27" s="1">
-        <v>8.64</v>
       </c>
       <c r="U27" s="1">
         <v>8.64</v>
       </c>
-    </row>
-    <row r="28" spans="2:21" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="V27" s="1">
+        <v>8.64</v>
+      </c>
+    </row>
+    <row r="28" spans="1:22" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B28" s="1" t="s">
         <v>117</v>
       </c>
@@ -1992,18 +2029,76 @@
       <c r="Q28" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="R28" s="1">
-        <v>1</v>
-      </c>
-      <c r="T28" s="1">
-        <v>59</v>
+      <c r="R28" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="S28" s="1">
+        <v>1</v>
       </c>
       <c r="U28" s="1">
         <v>59</v>
       </c>
-    </row>
-    <row r="29" spans="2:21" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E29" s="8"/>
+      <c r="V28" s="1">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="29" spans="1:22" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B29" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="C29" s="1">
+        <v>1</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="E29" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="Q29" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="R29" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="S29" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="U29" s="1">
+        <v>3.12</v>
+      </c>
+      <c r="V29" s="1">
+        <v>3.12</v>
+      </c>
+    </row>
+    <row r="30" spans="1:22" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B30" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="C30" s="1">
+        <v>1</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="Q30" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="R30" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="S30" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="U30" s="1">
+        <v>3.45</v>
+      </c>
+      <c r="V30" s="1">
+        <v>3.45</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
@@ -2014,6 +2109,9 @@
     <hyperlink ref="F5" display="http://za.rs-online.com/web/p/microcontrollers/7618633/?searchTerm=stm32f051c6t&amp;relevancy-data=636F3D3526696E3D4931384E4D616E506172744E756D626572266C753D656E266D6D3D6D61746368616C6C7061727469616C26706D3D5E5B5C707B4C7D5C707B4E647D2D2C2F255C2E5D2B2426706F3D"/>
     <hyperlink ref="F7" r:id="rId5"/>
     <hyperlink ref="F9" r:id="rId6"/>
+    <hyperlink ref="R28" r:id="rId7"/>
+    <hyperlink ref="R29" r:id="rId8"/>
+    <hyperlink ref="R30" r:id="rId9"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added website and started stm code
website foreground mostly done
started with st code
</commit_message>
<xml_diff>
--- a/Circuit/Part List.xlsx
+++ b/Circuit/Part List.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9735" firstSheet="1" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9735"/>
   </bookViews>
   <sheets>
     <sheet name="Packages" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="188">
   <si>
     <t>component</t>
   </si>
@@ -588,13 +588,16 @@
   </si>
   <si>
     <t>Series 5556 4.2 pitch 20 way</t>
+  </si>
+  <si>
+    <t>height</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -649,6 +652,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1" tint="0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -940,12 +951,9 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="3" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="3" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="2" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="4" applyFill="1" applyBorder="1"/>
@@ -985,6 +993,8 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="4" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="4" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="4" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="3" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="3" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -1269,10 +1279,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F29"/>
+  <dimension ref="A1:J30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18:XFD18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" thickTop="1" thickBottom="1" x14ac:dyDescent="0.3"/>
@@ -1281,10 +1291,12 @@
     <col min="2" max="2" width="36.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="1"/>
+    <col min="5" max="5" width="9.140625" style="1"/>
+    <col min="6" max="6" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1297,8 +1309,12 @@
       <c r="D1" s="1" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E1" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="F1" s="37"/>
+    </row>
+    <row r="2" spans="1:10" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -1308,9 +1324,23 @@
       <c r="D2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="2"/>
-    </row>
-    <row r="3" spans="1:6" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E2" s="1">
+        <v>9.6</v>
+      </c>
+      <c r="F2" s="37">
+        <v>10.66</v>
+      </c>
+      <c r="G2" s="1">
+        <v>10.16</v>
+      </c>
+      <c r="H2" s="1">
+        <v>10.82</v>
+      </c>
+      <c r="I2" s="1">
+        <v>10.16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -1323,9 +1353,26 @@
       <c r="D3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="2"/>
-    </row>
-    <row r="4" spans="1:6" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E3" s="1">
+        <v>20</v>
+      </c>
+      <c r="F3" s="37">
+        <v>19.5</v>
+      </c>
+      <c r="G3" s="1">
+        <v>20.190000000000001</v>
+      </c>
+      <c r="H3" s="1">
+        <v>19.559999999999999</v>
+      </c>
+      <c r="I3" s="1">
+        <v>20.32</v>
+      </c>
+      <c r="J3" s="1">
+        <v>19.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
@@ -1336,11 +1383,25 @@
         <v>12</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F4" s="2"/>
-    </row>
-    <row r="5" spans="1:6" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>37</v>
+      </c>
+      <c r="E4" s="1">
+        <v>19.55</v>
+      </c>
+      <c r="F4" s="37">
+        <v>20.32</v>
+      </c>
+      <c r="G4" s="1">
+        <v>19.5</v>
+      </c>
+      <c r="H4" s="1">
+        <v>21.97</v>
+      </c>
+      <c r="I4" s="1">
+        <v>19.809999999999999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
@@ -1351,11 +1412,22 @@
         <v>11</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="F5" s="2"/>
-    </row>
-    <row r="6" spans="1:6" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>38</v>
+      </c>
+      <c r="E5" s="1">
+        <v>25.73</v>
+      </c>
+      <c r="F5" s="37">
+        <v>26.42</v>
+      </c>
+      <c r="G5" s="1">
+        <v>27.17</v>
+      </c>
+      <c r="H5" s="1">
+        <v>25.4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
@@ -1366,11 +1438,11 @@
         <v>12</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="F6" s="2"/>
-    </row>
-    <row r="7" spans="1:6" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>39</v>
+      </c>
+      <c r="F6" s="37"/>
+    </row>
+    <row r="7" spans="1:10" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
@@ -1378,11 +1450,11 @@
         <v>15</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="F7" s="2"/>
-    </row>
-    <row r="8" spans="1:6" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>43</v>
+      </c>
+      <c r="F7" s="37"/>
+    </row>
+    <row r="8" spans="1:10" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>9</v>
       </c>
@@ -1393,11 +1465,11 @@
         <v>11</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="F8" s="2"/>
-    </row>
-    <row r="9" spans="1:6" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>44</v>
+      </c>
+      <c r="F8" s="37"/>
+    </row>
+    <row r="9" spans="1:10" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>10</v>
       </c>
@@ -1408,11 +1480,11 @@
         <v>12</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="F9" s="2"/>
-    </row>
-    <row r="10" spans="1:6" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>46</v>
+      </c>
+      <c r="F9" s="37"/>
+    </row>
+    <row r="10" spans="1:10" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B10" s="1" t="s">
         <v>16</v>
       </c>
@@ -1420,11 +1492,11 @@
         <v>37</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="F10" s="2"/>
-    </row>
-    <row r="11" spans="1:6" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>49</v>
+      </c>
+      <c r="F10" s="37"/>
+    </row>
+    <row r="11" spans="1:10" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B11" s="1" t="s">
         <v>55</v>
       </c>
@@ -1432,11 +1504,11 @@
         <v>38</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="F11" s="2"/>
-    </row>
-    <row r="12" spans="1:6" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>50</v>
+      </c>
+      <c r="F11" s="37"/>
+    </row>
+    <row r="12" spans="1:10" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>17</v>
       </c>
@@ -1446,12 +1518,9 @@
       <c r="C12" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D12" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="F12" s="2"/>
-    </row>
-    <row r="13" spans="1:6" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F12" s="37"/>
+    </row>
+    <row r="13" spans="1:10" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>18</v>
       </c>
@@ -1461,9 +1530,9 @@
       <c r="C13" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="F13" s="2"/>
-    </row>
-    <row r="14" spans="1:6" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F13" s="37"/>
+    </row>
+    <row r="14" spans="1:10" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>19</v>
       </c>
@@ -1473,9 +1542,9 @@
       <c r="C14" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="F14" s="2"/>
-    </row>
-    <row r="15" spans="1:6" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F14" s="37"/>
+    </row>
+    <row r="15" spans="1:10" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>20</v>
       </c>
@@ -1485,9 +1554,9 @@
       <c r="C15" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="F15" s="2"/>
-    </row>
-    <row r="16" spans="1:6" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F15" s="37"/>
+    </row>
+    <row r="16" spans="1:10" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>45</v>
       </c>
@@ -1497,7 +1566,7 @@
       <c r="C16" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="F16" s="2"/>
+      <c r="F16" s="37"/>
     </row>
     <row r="17" spans="1:6" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
@@ -1509,7 +1578,7 @@
       <c r="C17" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="F17" s="2"/>
+      <c r="F17" s="37"/>
     </row>
     <row r="18" spans="1:6" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
@@ -1521,7 +1590,7 @@
       <c r="C18" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="F18" s="2"/>
+      <c r="F18" s="37"/>
     </row>
     <row r="19" spans="1:6" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
@@ -1533,7 +1602,7 @@
       <c r="C19" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="F19" s="2"/>
+      <c r="F19" s="37"/>
     </row>
     <row r="20" spans="1:6" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
@@ -1545,7 +1614,7 @@
       <c r="C20" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="F20" s="2"/>
+      <c r="F20" s="37"/>
     </row>
     <row r="21" spans="1:6" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
@@ -1554,7 +1623,7 @@
       <c r="C21" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="F21" s="2"/>
+      <c r="F21" s="37"/>
     </row>
     <row r="22" spans="1:6" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
@@ -1563,7 +1632,7 @@
       <c r="C22" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="F22" s="2"/>
+      <c r="F22" s="37"/>
     </row>
     <row r="23" spans="1:6" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
@@ -1572,7 +1641,7 @@
       <c r="C23" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="F23" s="2"/>
+      <c r="F23" s="37"/>
     </row>
     <row r="24" spans="1:6" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
@@ -1581,7 +1650,7 @@
       <c r="C24" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="F24" s="2"/>
+      <c r="F24" s="37"/>
     </row>
     <row r="25" spans="1:6" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
@@ -1590,7 +1659,7 @@
       <c r="C25" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="F25" s="2"/>
+      <c r="F25" s="37"/>
     </row>
     <row r="26" spans="1:6" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
@@ -1602,7 +1671,7 @@
       <c r="C26" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F26" s="2"/>
+      <c r="F26" s="37"/>
     </row>
     <row r="27" spans="1:6" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
@@ -1614,7 +1683,7 @@
       <c r="C27" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F27" s="2"/>
+      <c r="F27" s="37"/>
     </row>
     <row r="28" spans="1:6" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
@@ -1626,10 +1695,13 @@
       <c r="C28" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F28" s="2"/>
+      <c r="F28" s="37"/>
     </row>
     <row r="29" spans="1:6" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F29" s="2"/>
+      <c r="F29" s="37"/>
+    </row>
+    <row r="30" spans="1:6" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F30" s="38"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1664,10 +1736,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:23" ht="24.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="C2" s="3"/>
+      <c r="C2" s="2"/>
       <c r="G2" s="1" t="s">
         <v>89</v>
       </c>
@@ -1691,7 +1763,7 @@
       <c r="D4" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="E4" s="7" t="s">
+      <c r="E4" s="6" t="s">
         <v>67</v>
       </c>
       <c r="F4" s="1" t="s">
@@ -1759,21 +1831,21 @@
       <c r="D5" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="E5" s="7" t="s">
+      <c r="E5" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="F5" s="6" t="s">
+      <c r="F5" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="G5" s="4">
+      <c r="G5" s="3">
         <v>0</v>
       </c>
-      <c r="H5" s="4" t="s">
+      <c r="H5" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="I5" s="4"/>
-      <c r="J5" s="4"/>
-      <c r="K5" s="5" t="s">
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
+      <c r="K5" s="4" t="s">
         <v>70</v>
       </c>
       <c r="L5" s="1">
@@ -1801,10 +1873,10 @@
       <c r="D6" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="E6" s="7" t="s">
+      <c r="E6" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="F6" s="5" t="s">
+      <c r="F6" s="4" t="s">
         <v>75</v>
       </c>
       <c r="G6" s="1">
@@ -1817,7 +1889,7 @@
         <f>H6/G6</f>
         <v>8.9659999999999993</v>
       </c>
-      <c r="K6" s="5" t="s">
+      <c r="K6" s="4" t="s">
         <v>73</v>
       </c>
       <c r="L6" s="1">
@@ -1842,10 +1914,10 @@
       <c r="C7" s="1">
         <v>1</v>
       </c>
-      <c r="E7" s="7" t="s">
+      <c r="E7" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="F7" s="5" t="s">
+      <c r="F7" s="4" t="s">
         <v>78</v>
       </c>
       <c r="G7" s="1">
@@ -1858,7 +1930,7 @@
         <f t="shared" ref="I7:I28" si="2">H7/G7</f>
         <v>2.9820000000000002</v>
       </c>
-      <c r="K7" s="5" t="s">
+      <c r="K7" s="4" t="s">
         <v>90</v>
       </c>
       <c r="L7" s="1">
@@ -1886,11 +1958,11 @@
       <c r="D8" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="E8" s="7">
+      <c r="E8" s="6">
         <v>805</v>
       </c>
-      <c r="F8" s="5"/>
-      <c r="K8" s="5"/>
+      <c r="F8" s="4"/>
+      <c r="K8" s="4"/>
     </row>
     <row r="9" spans="2:23" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B9" s="1" t="s">
@@ -1902,10 +1974,10 @@
       <c r="D9" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="E9" s="7">
+      <c r="E9" s="6">
         <v>805</v>
       </c>
-      <c r="F9" s="5" t="s">
+      <c r="F9" s="4" t="s">
         <v>86</v>
       </c>
       <c r="G9" s="1">
@@ -1918,7 +1990,7 @@
         <f t="shared" si="2"/>
         <v>0.13100000000000001</v>
       </c>
-      <c r="K9" s="5" t="s">
+      <c r="K9" s="4" t="s">
         <v>79</v>
       </c>
       <c r="L9" s="1">
@@ -1946,7 +2018,7 @@
       <c r="D10" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="E10" s="7" t="s">
+      <c r="E10" s="6" t="s">
         <v>94</v>
       </c>
       <c r="F10" s="1" t="s">
@@ -1990,7 +2062,7 @@
       <c r="D11" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="E11" s="7" t="s">
+      <c r="E11" s="6" t="s">
         <v>97</v>
       </c>
       <c r="I11" s="1" t="e">
@@ -2025,7 +2097,7 @@
       <c r="D12" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="E12" s="7" t="s">
+      <c r="E12" s="6" t="s">
         <v>129</v>
       </c>
       <c r="I12" s="1" t="e">
@@ -2060,7 +2132,7 @@
       <c r="D13" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="E13" s="7">
+      <c r="E13" s="6">
         <v>805</v>
       </c>
       <c r="I13" s="1" t="e">
@@ -2086,7 +2158,7 @@
       <c r="D14" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="E14" s="7">
+      <c r="E14" s="6">
         <v>805</v>
       </c>
       <c r="I14" s="1" t="e">
@@ -2109,7 +2181,7 @@
       <c r="C15" s="1">
         <v>1</v>
       </c>
-      <c r="E15" s="7">
+      <c r="E15" s="6">
         <v>1206</v>
       </c>
       <c r="I15" s="1" t="e">
@@ -2132,7 +2204,7 @@
       <c r="C16" s="1">
         <v>1</v>
       </c>
-      <c r="E16" s="7">
+      <c r="E16" s="6">
         <v>1206</v>
       </c>
       <c r="I16" s="1" t="e">
@@ -2155,7 +2227,7 @@
       <c r="C17" s="1">
         <v>1</v>
       </c>
-      <c r="E17" s="7">
+      <c r="E17" s="6">
         <v>1206</v>
       </c>
       <c r="I17" s="1" t="e">
@@ -2181,7 +2253,7 @@
       <c r="D18" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="E18" s="7">
+      <c r="E18" s="6">
         <v>805</v>
       </c>
       <c r="I18" s="1" t="e">
@@ -2207,7 +2279,7 @@
       <c r="D19" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="E19" s="7">
+      <c r="E19" s="6">
         <v>805</v>
       </c>
       <c r="I19" s="1" t="e">
@@ -2233,7 +2305,7 @@
       <c r="D20" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="E20" s="7">
+      <c r="E20" s="6">
         <v>805</v>
       </c>
       <c r="I20" s="1" t="e">
@@ -2255,7 +2327,7 @@
       <c r="D21" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="E21" s="7">
+      <c r="E21" s="6">
         <v>805</v>
       </c>
       <c r="I21" s="1" t="e">
@@ -2277,7 +2349,7 @@
       <c r="D22" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="E22" s="7" t="s">
+      <c r="E22" s="6" t="s">
         <v>128</v>
       </c>
       <c r="I22" s="1" t="e">
@@ -2299,7 +2371,7 @@
       <c r="D23" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="E23" s="7" t="s">
+      <c r="E23" s="6" t="s">
         <v>128</v>
       </c>
       <c r="I23" s="1" t="e">
@@ -2321,7 +2393,7 @@
       <c r="D24" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="E24" s="7" t="s">
+      <c r="E24" s="6" t="s">
         <v>146</v>
       </c>
       <c r="I24" s="1" t="e">
@@ -2343,7 +2415,7 @@
       <c r="D25" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="E25" s="7" t="s">
+      <c r="E25" s="6" t="s">
         <v>128</v>
       </c>
       <c r="I25" s="1" t="e">
@@ -2365,7 +2437,7 @@
       <c r="D26" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="E26" s="7" t="s">
+      <c r="E26" s="6" t="s">
         <v>128</v>
       </c>
       <c r="I26" s="1" t="e">
@@ -2387,7 +2459,7 @@
       <c r="D27" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="E27" s="7" t="s">
+      <c r="E27" s="6" t="s">
         <v>128</v>
       </c>
       <c r="I27" s="1" t="e">
@@ -2458,7 +2530,7 @@
       <c r="D35" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="E35" s="7" t="s">
+      <c r="E35" s="6" t="s">
         <v>130</v>
       </c>
       <c r="Q35" s="1" t="s">
@@ -2484,13 +2556,13 @@
       <c r="D36" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="E36" s="7" t="s">
+      <c r="E36" s="6" t="s">
         <v>131</v>
       </c>
       <c r="Q36" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="R36" s="5" t="s">
+      <c r="R36" s="4" t="s">
         <v>137</v>
       </c>
       <c r="S36" s="1">
@@ -2513,13 +2585,13 @@
       <c r="D37" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="E37" s="8" t="s">
+      <c r="E37" s="7" t="s">
         <v>141</v>
       </c>
       <c r="Q37" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="R37" s="5" t="s">
+      <c r="R37" s="4" t="s">
         <v>142</v>
       </c>
       <c r="S37" s="1" t="s">
@@ -2548,7 +2620,7 @@
       <c r="Q38" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="R38" s="5" t="s">
+      <c r="R38" s="4" t="s">
         <v>144</v>
       </c>
       <c r="S38" s="1" t="s">
@@ -2582,7 +2654,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:H17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
@@ -2597,305 +2669,305 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="25" t="s">
+      <c r="B2" s="24" t="s">
         <v>165</v>
       </c>
     </row>
     <row r="3" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="9" t="s">
         <v>168</v>
       </c>
-      <c r="C3" s="14" t="s">
+      <c r="C3" s="13" t="s">
         <v>170</v>
       </c>
-      <c r="D3" s="10" t="s">
+      <c r="D3" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="E3" s="14" t="s">
+      <c r="E3" s="13" t="s">
         <v>167</v>
       </c>
-      <c r="F3" s="10" t="s">
+      <c r="F3" s="9" t="s">
         <v>182</v>
       </c>
-      <c r="G3" s="29" t="s">
+      <c r="G3" s="28" t="s">
         <v>169</v>
       </c>
-      <c r="H3" s="31" t="s">
+      <c r="H3" s="30" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B4" s="11" t="s">
+      <c r="B4" s="10" t="s">
         <v>176</v>
       </c>
-      <c r="C4" s="15">
-        <v>1</v>
-      </c>
-      <c r="D4" s="11" t="s">
+      <c r="C4" s="14">
+        <v>1</v>
+      </c>
+      <c r="D4" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="E4" s="33" t="s">
+      <c r="E4" s="32" t="s">
         <v>184</v>
       </c>
-      <c r="F4" s="20">
+      <c r="F4" s="19">
         <v>5</v>
       </c>
-      <c r="G4" s="15">
+      <c r="G4" s="14">
         <v>173.21</v>
       </c>
-      <c r="H4" s="11">
+      <c r="H4" s="10">
         <f>G4/F4</f>
         <v>34.642000000000003</v>
       </c>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B5" s="12" t="s">
+      <c r="B5" s="11" t="s">
         <v>71</v>
       </c>
-      <c r="C5" s="16">
-        <v>1</v>
-      </c>
-      <c r="D5" s="12" t="s">
+      <c r="C5" s="15">
+        <v>1</v>
+      </c>
+      <c r="D5" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="E5" s="34" t="s">
+      <c r="E5" s="33" t="s">
         <v>75</v>
       </c>
-      <c r="F5" s="12">
+      <c r="F5" s="11">
         <v>10</v>
       </c>
-      <c r="G5" s="16">
+      <c r="G5" s="15">
         <v>89.66</v>
       </c>
-      <c r="H5" s="11">
+      <c r="H5" s="10">
         <f t="shared" ref="H5:H10" si="0">G5/F5</f>
         <v>8.9659999999999993</v>
       </c>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B6" s="12" t="s">
+      <c r="B6" s="11" t="s">
         <v>76</v>
       </c>
-      <c r="C6" s="16">
-        <v>1</v>
-      </c>
-      <c r="D6" s="12" t="s">
+      <c r="C6" s="15">
+        <v>1</v>
+      </c>
+      <c r="D6" s="11" t="s">
         <v>77</v>
       </c>
-      <c r="E6" s="34" t="s">
+      <c r="E6" s="33" t="s">
         <v>171</v>
       </c>
-      <c r="F6" s="12">
+      <c r="F6" s="11">
         <v>5</v>
       </c>
-      <c r="G6" s="16">
+      <c r="G6" s="15">
         <v>21.79</v>
       </c>
-      <c r="H6" s="11">
+      <c r="H6" s="10">
         <f t="shared" si="0"/>
         <v>4.3579999999999997</v>
       </c>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B7" s="12" t="s">
+      <c r="B7" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="C7" s="16">
-        <v>1</v>
-      </c>
-      <c r="D7" s="12" t="s">
+      <c r="C7" s="15">
+        <v>1</v>
+      </c>
+      <c r="D7" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="E7" s="34" t="s">
+      <c r="E7" s="33" t="s">
         <v>98</v>
       </c>
-      <c r="F7" s="12">
+      <c r="F7" s="11">
         <v>25</v>
       </c>
-      <c r="G7" s="16">
+      <c r="G7" s="15">
         <v>10.475</v>
       </c>
-      <c r="H7" s="11">
+      <c r="H7" s="10">
         <f t="shared" si="0"/>
         <v>0.41899999999999998</v>
       </c>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B8" s="12" t="s">
+      <c r="B8" s="11" t="s">
         <v>173</v>
       </c>
-      <c r="C8" s="16">
-        <v>1</v>
-      </c>
-      <c r="D8" s="12" t="s">
+      <c r="C8" s="15">
+        <v>1</v>
+      </c>
+      <c r="D8" s="11" t="s">
         <v>97</v>
       </c>
-      <c r="E8" s="34" t="s">
+      <c r="E8" s="33" t="s">
         <v>172</v>
       </c>
-      <c r="F8" s="12">
+      <c r="F8" s="11">
         <v>10</v>
       </c>
-      <c r="G8" s="16">
+      <c r="G8" s="15">
         <v>20.51</v>
       </c>
-      <c r="H8" s="11">
+      <c r="H8" s="10">
         <f t="shared" si="0"/>
         <v>2.0510000000000002</v>
       </c>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B9" s="12" t="s">
+      <c r="B9" s="11" t="s">
         <v>175</v>
       </c>
-      <c r="C9" s="16">
-        <v>1</v>
-      </c>
-      <c r="D9" s="12" t="s">
+      <c r="C9" s="15">
+        <v>1</v>
+      </c>
+      <c r="D9" s="11" t="s">
         <v>129</v>
       </c>
-      <c r="E9" s="34" t="s">
+      <c r="E9" s="33" t="s">
         <v>178</v>
       </c>
-      <c r="F9" s="12">
+      <c r="F9" s="11">
         <v>21</v>
       </c>
-      <c r="G9" s="16">
+      <c r="G9" s="15">
         <v>161.69999999999999</v>
       </c>
-      <c r="H9" s="11">
+      <c r="H9" s="10">
         <f t="shared" si="0"/>
         <v>7.6999999999999993</v>
       </c>
     </row>
     <row r="10" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="18" t="s">
+      <c r="B10" s="17" t="s">
         <v>164</v>
       </c>
-      <c r="C10" s="19">
-        <v>1</v>
-      </c>
-      <c r="D10" s="18" t="s">
+      <c r="C10" s="18">
+        <v>1</v>
+      </c>
+      <c r="D10" s="17" t="s">
         <v>131</v>
       </c>
-      <c r="E10" s="35" t="s">
+      <c r="E10" s="34" t="s">
         <v>137</v>
       </c>
-      <c r="F10" s="13">
-        <v>1</v>
-      </c>
-      <c r="G10" s="19">
+      <c r="F10" s="12">
+        <v>1</v>
+      </c>
+      <c r="G10" s="18">
         <v>59</v>
       </c>
-      <c r="H10" s="32">
+      <c r="H10" s="31">
         <f t="shared" si="0"/>
         <v>59</v>
       </c>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B11" s="20"/>
-      <c r="C11" s="20"/>
-      <c r="D11" s="20"/>
-      <c r="E11" s="28"/>
-      <c r="F11" s="20"/>
-      <c r="G11" s="28"/>
-      <c r="H11" s="11"/>
+      <c r="B11" s="19"/>
+      <c r="C11" s="19"/>
+      <c r="D11" s="19"/>
+      <c r="E11" s="27"/>
+      <c r="F11" s="19"/>
+      <c r="G11" s="27"/>
+      <c r="H11" s="10"/>
     </row>
     <row r="12" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="24" t="s">
+      <c r="B12" s="23" t="s">
         <v>166</v>
       </c>
-      <c r="C12" s="13"/>
-      <c r="D12" s="13"/>
-      <c r="E12" s="30"/>
-      <c r="F12" s="18"/>
-      <c r="G12" s="30"/>
-      <c r="H12" s="18"/>
+      <c r="C12" s="12"/>
+      <c r="D12" s="12"/>
+      <c r="E12" s="29"/>
+      <c r="F12" s="17"/>
+      <c r="G12" s="29"/>
+      <c r="H12" s="17"/>
     </row>
     <row r="13" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="27" t="s">
+      <c r="B13" s="26" t="s">
         <v>168</v>
       </c>
-      <c r="C13" s="26" t="s">
+      <c r="C13" s="25" t="s">
         <v>119</v>
       </c>
-      <c r="D13" s="29" t="s">
+      <c r="D13" s="28" t="s">
         <v>67</v>
       </c>
-      <c r="E13" s="29" t="s">
+      <c r="E13" s="28" t="s">
         <v>167</v>
       </c>
-      <c r="F13" s="10" t="s">
+      <c r="F13" s="9" t="s">
         <v>182</v>
       </c>
-      <c r="G13" s="29" t="s">
+      <c r="G13" s="28" t="s">
         <v>169</v>
       </c>
-      <c r="H13" s="10" t="s">
+      <c r="H13" s="9" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B14" s="21" t="s">
+      <c r="B14" s="20" t="s">
         <v>177</v>
       </c>
-      <c r="C14" s="20">
-        <v>1</v>
-      </c>
-      <c r="D14" s="15" t="s">
+      <c r="C14" s="19">
+        <v>1</v>
+      </c>
+      <c r="D14" s="14" t="s">
         <v>154</v>
       </c>
-      <c r="E14" s="36" t="s">
+      <c r="E14" s="35" t="s">
         <v>181</v>
       </c>
-      <c r="F14" s="11">
+      <c r="F14" s="10">
         <v>5</v>
       </c>
-      <c r="G14" s="21">
+      <c r="G14" s="20">
         <v>113.54</v>
       </c>
-      <c r="H14" s="11">
+      <c r="H14" s="10">
         <f t="shared" ref="H14:H16" si="1">G14/F14</f>
         <v>22.708000000000002</v>
       </c>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B15" s="22" t="s">
+      <c r="B15" s="21" t="s">
         <v>71</v>
       </c>
-      <c r="C15" s="12">
-        <v>1</v>
-      </c>
-      <c r="D15" s="16" t="s">
+      <c r="C15" s="11">
+        <v>1</v>
+      </c>
+      <c r="D15" s="15" t="s">
         <v>72</v>
       </c>
-      <c r="E15" s="22"/>
-      <c r="F15" s="12" t="s">
+      <c r="E15" s="21"/>
+      <c r="F15" s="11" t="s">
         <v>179</v>
       </c>
-      <c r="G15" s="22"/>
-      <c r="H15" s="11"/>
+      <c r="G15" s="21"/>
+      <c r="H15" s="10"/>
     </row>
     <row r="16" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="23" t="s">
+      <c r="B16" s="22" t="s">
         <v>185</v>
       </c>
-      <c r="C16" s="13">
-        <v>1</v>
-      </c>
-      <c r="D16" s="17" t="s">
+      <c r="C16" s="12">
+        <v>1</v>
+      </c>
+      <c r="D16" s="16" t="s">
         <v>186</v>
       </c>
-      <c r="E16" s="37" t="s">
+      <c r="E16" s="36" t="s">
         <v>180</v>
       </c>
-      <c r="F16" s="13">
+      <c r="F16" s="12">
         <v>5</v>
       </c>
-      <c r="G16" s="23">
+      <c r="G16" s="22">
         <v>91.48</v>
       </c>
-      <c r="H16" s="32">
+      <c r="H16" s="31">
         <f t="shared" si="1"/>
         <v>18.295999999999999</v>
       </c>
@@ -2952,10 +3024,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:23" ht="24.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="C2" s="3"/>
+      <c r="C2" s="2"/>
       <c r="G2" s="1" t="s">
         <v>89</v>
       </c>
@@ -2979,7 +3051,7 @@
       <c r="D4" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="E4" s="7" t="s">
+      <c r="E4" s="6" t="s">
         <v>67</v>
       </c>
       <c r="F4" s="1" t="s">
@@ -3047,15 +3119,15 @@
       <c r="D5" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="E5" s="7" t="s">
+      <c r="E5" s="6" t="s">
         <v>128</v>
       </c>
-      <c r="F5" s="9"/>
-      <c r="G5" s="9"/>
-      <c r="H5" s="9"/>
-      <c r="I5" s="9"/>
-      <c r="J5" s="9"/>
-      <c r="K5" s="5"/>
+      <c r="F5" s="8"/>
+      <c r="G5" s="8"/>
+      <c r="H5" s="8"/>
+      <c r="I5" s="8"/>
+      <c r="J5" s="8"/>
+      <c r="K5" s="4"/>
       <c r="O5" s="1" t="e">
         <f>N5/L5</f>
         <v>#DIV/0!</v>
@@ -3074,10 +3146,10 @@
       <c r="D6" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="E6" s="7" t="s">
+      <c r="E6" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="F6" s="5" t="s">
+      <c r="F6" s="4" t="s">
         <v>75</v>
       </c>
       <c r="G6" s="1">
@@ -3090,7 +3162,7 @@
         <f>H6/G6</f>
         <v>8.9659999999999993</v>
       </c>
-      <c r="K6" s="5" t="s">
+      <c r="K6" s="4" t="s">
         <v>73</v>
       </c>
       <c r="L6" s="1">
@@ -3121,7 +3193,7 @@
       <c r="D7" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="E7" s="7" t="s">
+      <c r="E7" s="6" t="s">
         <v>146</v>
       </c>
       <c r="I7" s="1" t="e">
@@ -3143,7 +3215,7 @@
       <c r="C8" s="1">
         <v>1</v>
       </c>
-      <c r="E8" s="7">
+      <c r="E8" s="6">
         <v>1206</v>
       </c>
       <c r="I8" s="1" t="e">
@@ -3172,7 +3244,7 @@
       <c r="D9" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="E9" s="7">
+      <c r="E9" s="6">
         <v>805</v>
       </c>
       <c r="I9" s="1" t="e">
@@ -3201,7 +3273,7 @@
       <c r="D10" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="E10" s="7">
+      <c r="E10" s="6">
         <v>805</v>
       </c>
       <c r="I10" s="1" t="e">
@@ -3227,15 +3299,15 @@
       <c r="D11" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="E11" s="7" t="s">
+      <c r="E11" s="6" t="s">
         <v>158</v>
       </c>
       <c r="I11" s="1" t="e">
-        <f t="shared" ref="I7:I28" si="4">H11/G11</f>
+        <f t="shared" ref="I11" si="4">H11/G11</f>
         <v>#DIV/0!</v>
       </c>
       <c r="O11" s="1" t="e">
-        <f t="shared" ref="O6:O28" si="5">N11/L11</f>
+        <f t="shared" ref="O11" si="5">N11/L11</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -3246,7 +3318,7 @@
       <c r="C12" s="1">
         <v>6</v>
       </c>
-      <c r="E12" s="7" t="s">
+      <c r="E12" s="6" t="s">
         <v>161</v>
       </c>
     </row>
@@ -3257,65 +3329,65 @@
       <c r="C13" s="1">
         <v>3</v>
       </c>
-      <c r="E13" s="7" t="s">
+      <c r="E13" s="6" t="s">
         <v>161</v>
       </c>
     </row>
     <row r="14" spans="1:23" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E14" s="7"/>
+      <c r="E14" s="6"/>
     </row>
     <row r="15" spans="1:23" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E15" s="7"/>
+      <c r="E15" s="6"/>
     </row>
     <row r="16" spans="1:23" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E16" s="7"/>
+      <c r="E16" s="6"/>
     </row>
     <row r="17" spans="5:5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E17" s="7"/>
+      <c r="E17" s="6"/>
     </row>
     <row r="18" spans="5:5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E18" s="7"/>
+      <c r="E18" s="6"/>
     </row>
     <row r="19" spans="5:5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E19" s="7"/>
+      <c r="E19" s="6"/>
     </row>
     <row r="20" spans="5:5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E20" s="7"/>
+      <c r="E20" s="6"/>
     </row>
     <row r="21" spans="5:5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E21" s="7"/>
+      <c r="E21" s="6"/>
     </row>
     <row r="22" spans="5:5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E22" s="7"/>
+      <c r="E22" s="6"/>
     </row>
     <row r="23" spans="5:5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E23" s="7"/>
+      <c r="E23" s="6"/>
     </row>
     <row r="24" spans="5:5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E24" s="7"/>
+      <c r="E24" s="6"/>
     </row>
     <row r="25" spans="5:5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E25" s="7"/>
+      <c r="E25" s="6"/>
     </row>
     <row r="26" spans="5:5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E26" s="7"/>
+      <c r="E26" s="6"/>
     </row>
     <row r="27" spans="5:5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E27" s="7"/>
+      <c r="E27" s="6"/>
     </row>
     <row r="35" spans="5:18" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E35" s="7"/>
+      <c r="E35" s="6"/>
     </row>
     <row r="36" spans="5:18" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E36" s="7"/>
-      <c r="R36" s="5"/>
+      <c r="E36" s="6"/>
+      <c r="R36" s="4"/>
     </row>
     <row r="37" spans="5:18" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E37" s="8"/>
-      <c r="R37" s="5"/>
+      <c r="E37" s="7"/>
+      <c r="R37" s="4"/>
     </row>
     <row r="38" spans="5:18" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="R38" s="5"/>
+      <c r="R38" s="4"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>